<commit_message>
adding listenets to testng.xml and creating TestUtils.class (captureScreenshot methot)
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/testData.xlsx
+++ b/src/main/resources/excel/testData.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anicolle\eclipse-workspace\DataDrivenFramework\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A47CD274-2F1C-4B1C-A435-8DBAABA975B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B06F8F3-7AD2-408B-B525-574E294E50E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{8BAA97C8-049B-4362-B615-43A6A114C06F}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="7460" xr2:uid="{8BAA97C8-049B-4362-B615-43A6A114C06F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,15 +33,50 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>postCode</t>
+  </si>
+  <si>
+    <t>Anne</t>
+  </si>
+  <si>
+    <t>Zimmermann</t>
+  </si>
+  <si>
+    <t>89046-305</t>
+  </si>
+  <si>
+    <t>alertText</t>
+  </si>
+  <si>
+    <t>Customer added successfully</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -64,8 +99,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,12 +418,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE5E80B4-9AE9-44E6-AD2D-52301B40F741}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
creating common data provider and adding log4j how logger
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/testData.xlsx
+++ b/src/main/resources/excel/testData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anicolle\eclipse-workspace\DataDrivenFramework\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B06F8F3-7AD2-408B-B525-574E294E50E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09029A1-8B36-4B9A-8246-2CA2EDBF68EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="7460" xr2:uid="{8BAA97C8-049B-4362-B615-43A6A114C06F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{8BAA97C8-049B-4362-B615-43A6A114C06F}"/>
   </bookViews>
   <sheets>
-    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
+    <sheet name="ADDCUSTOMER" sheetId="1" r:id="rId1"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>firstName</t>
   </si>
@@ -58,6 +59,18 @@
   </si>
   <si>
     <t>Customer added successfully</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>Anne Zimmermann</t>
+  </si>
+  <si>
+    <t>Real</t>
   </si>
 </sst>
 </file>
@@ -421,7 +434,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -464,4 +477,38 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACADF403-4737-4DD0-8D26-5E24A9AA5278}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>